<commit_message>
Initial plan for GC-corrected 22-subclass analysis
Co-authored-by: VRYella <67261325+VRYella@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Table4_Subclass_Distribution.xlsx
+++ b/Table4_Subclass_Distribution.xlsx
@@ -831,47 +831,47 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>B. aphidicola</t>
+          <t>Ca. Carsonella</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C2" t="n">
-        <v>583</v>
+        <v>270</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>2406</v>
+        <v>976</v>
       </c>
       <c r="F2" t="n">
-        <v>135</v>
+        <v>23</v>
       </c>
       <c r="G2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H2" t="n">
-        <v>265</v>
+        <v>117</v>
       </c>
       <c r="I2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M2" t="n">
         <v>0</v>
       </c>
       <c r="N2" t="n">
-        <v>79</v>
+        <v>11</v>
       </c>
       <c r="O2" t="n">
         <v>0</v>
@@ -883,53 +883,53 @@
         <v>0</v>
       </c>
       <c r="R2" t="n">
+        <v>1</v>
+      </c>
+      <c r="S2" t="n">
+        <v>18</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>22</v>
+      </c>
+      <c r="AG2" t="n">
         <v>25</v>
       </c>
-      <c r="S2" t="n">
-        <v>126</v>
-      </c>
-      <c r="T2" t="n">
-        <v>1</v>
-      </c>
-      <c r="U2" t="n">
-        <v>0</v>
-      </c>
-      <c r="V2" t="n">
-        <v>0</v>
-      </c>
-      <c r="W2" t="n">
-        <v>0</v>
-      </c>
-      <c r="X2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF2" t="n">
-        <v>42</v>
-      </c>
-      <c r="AG2" t="n">
-        <v>33</v>
-      </c>
       <c r="AH2" t="n">
         <v>0</v>
       </c>
@@ -943,7 +943,7 @@
         <v>0</v>
       </c>
       <c r="AL2" t="n">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="AM2" t="n">
         <v>0</v>
@@ -952,13 +952,13 @@
         <v>0</v>
       </c>
       <c r="AO2" t="n">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="AP2" t="n">
         <v>0</v>
       </c>
       <c r="AQ2" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AR2" t="n">
         <v>0</v>
@@ -970,7 +970,7 @@
         <v>0</v>
       </c>
       <c r="AU2" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AV2" t="n">
         <v>0</v>
@@ -982,10 +982,10 @@
         <v>0</v>
       </c>
       <c r="AY2" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="AZ2" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="BA2" t="n">
         <v>0</v>
@@ -997,7 +997,7 @@
         <v>0</v>
       </c>
       <c r="BD2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BE2" t="n">
         <v>0</v>
@@ -1021,7 +1021,7 @@
         <v>0</v>
       </c>
       <c r="BL2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BM2" t="n">
         <v>0</v>
@@ -1042,7 +1042,7 @@
         <v>0</v>
       </c>
       <c r="BS2" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BT2" t="n">
         <v>0</v>
@@ -1066,7 +1066,7 @@
         <v>0</v>
       </c>
       <c r="CA2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB2" t="n">
         <v>0</v>
@@ -1081,219 +1081,219 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Ca. Carsonella</t>
+          <t>B. aphidicola</t>
         </is>
       </c>
       <c r="B3" t="n">
+        <v>15</v>
+      </c>
+      <c r="C3" t="n">
+        <v>583</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>2406</v>
+      </c>
+      <c r="F3" t="n">
+        <v>135</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" t="n">
+        <v>265</v>
+      </c>
+      <c r="I3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" t="n">
+        <v>40</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>79</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" t="n">
+        <v>25</v>
+      </c>
+      <c r="S3" t="n">
+        <v>126</v>
+      </c>
+      <c r="T3" t="n">
+        <v>1</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W3" t="n">
+        <v>0</v>
+      </c>
+      <c r="X3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>42</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>33</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL3" t="n">
+        <v>26</v>
+      </c>
+      <c r="AM3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO3" t="n">
+        <v>22</v>
+      </c>
+      <c r="AP3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ3" t="n">
+        <v>3</v>
+      </c>
+      <c r="AR3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AV3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY3" t="n">
         <v>9</v>
       </c>
-      <c r="C3" t="n">
-        <v>270</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" t="n">
-        <v>976</v>
-      </c>
-      <c r="F3" t="n">
-        <v>23</v>
-      </c>
-      <c r="G3" t="n">
+      <c r="AZ3" t="n">
+        <v>7</v>
+      </c>
+      <c r="BA3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD3" t="n">
+        <v>3</v>
+      </c>
+      <c r="BE3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL3" t="n">
         <v>2</v>
       </c>
-      <c r="H3" t="n">
-        <v>117</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" t="n">
+      <c r="BM3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BR3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS3" t="n">
         <v>3</v>
       </c>
-      <c r="L3" t="n">
-        <v>1</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N3" t="n">
-        <v>11</v>
-      </c>
-      <c r="O3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R3" t="n">
-        <v>1</v>
-      </c>
-      <c r="S3" t="n">
-        <v>18</v>
-      </c>
-      <c r="T3" t="n">
-        <v>0</v>
-      </c>
-      <c r="U3" t="n">
-        <v>0</v>
-      </c>
-      <c r="V3" t="n">
-        <v>0</v>
-      </c>
-      <c r="W3" t="n">
-        <v>0</v>
-      </c>
-      <c r="X3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF3" t="n">
-        <v>22</v>
-      </c>
-      <c r="AG3" t="n">
-        <v>25</v>
-      </c>
-      <c r="AH3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL3" t="n">
-        <v>4</v>
-      </c>
-      <c r="AM3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO3" t="n">
-        <v>6</v>
-      </c>
-      <c r="AP3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AV3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AZ3" t="n">
-        <v>1</v>
-      </c>
-      <c r="BA3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD3" t="n">
-        <v>2</v>
-      </c>
-      <c r="BE3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BF3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BG3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BH3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BI3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BJ3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BK3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BL3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BM3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BN3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BO3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BP3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BQ3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BR3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BS3" t="n">
-        <v>0</v>
-      </c>
       <c r="BT3" t="n">
         <v>0</v>
       </c>
@@ -1316,7 +1316,7 @@
         <v>0</v>
       </c>
       <c r="CA3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CB3" t="n">
         <v>0</v>
@@ -1331,194 +1331,194 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>C. shaoxiangyii</t>
+          <t>H. pylori</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>20456</v>
+        <v>912</v>
       </c>
       <c r="C4" t="n">
-        <v>4947</v>
+        <v>476</v>
       </c>
       <c r="D4" t="n">
-        <v>8552</v>
+        <v>22</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>420</v>
       </c>
       <c r="F4" t="n">
-        <v>2991</v>
+        <v>82</v>
       </c>
       <c r="G4" t="n">
-        <v>1621</v>
+        <v>773</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>621</v>
       </c>
       <c r="I4" t="n">
-        <v>1814</v>
+        <v>22</v>
       </c>
       <c r="J4" t="n">
-        <v>1524</v>
+        <v>55</v>
       </c>
       <c r="K4" t="n">
-        <v>1258</v>
+        <v>25</v>
       </c>
       <c r="L4" t="n">
-        <v>987</v>
+        <v>108</v>
       </c>
       <c r="M4" t="n">
-        <v>803</v>
+        <v>54</v>
       </c>
       <c r="N4" t="n">
-        <v>306</v>
+        <v>54</v>
       </c>
       <c r="O4" t="n">
-        <v>484</v>
+        <v>16</v>
       </c>
       <c r="P4" t="n">
-        <v>394</v>
+        <v>2</v>
       </c>
       <c r="Q4" t="n">
-        <v>301</v>
+        <v>2</v>
       </c>
       <c r="R4" t="n">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="S4" t="n">
+        <v>14</v>
+      </c>
+      <c r="T4" t="n">
+        <v>2</v>
+      </c>
+      <c r="U4" t="n">
+        <v>1</v>
+      </c>
+      <c r="V4" t="n">
+        <v>8</v>
+      </c>
+      <c r="W4" t="n">
+        <v>5</v>
+      </c>
+      <c r="X4" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>6</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>6</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>6</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>6</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI4" t="n">
         <v>4</v>
       </c>
-      <c r="T4" t="n">
-        <v>262</v>
-      </c>
-      <c r="U4" t="n">
-        <v>188</v>
-      </c>
-      <c r="V4" t="n">
-        <v>193</v>
-      </c>
-      <c r="W4" t="n">
-        <v>145</v>
-      </c>
-      <c r="X4" t="n">
-        <v>103</v>
-      </c>
-      <c r="Y4" t="n">
-        <v>117</v>
-      </c>
-      <c r="Z4" t="n">
-        <v>122</v>
-      </c>
-      <c r="AA4" t="n">
-        <v>91</v>
-      </c>
-      <c r="AB4" t="n">
-        <v>81</v>
-      </c>
-      <c r="AC4" t="n">
-        <v>102</v>
-      </c>
-      <c r="AD4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE4" t="n">
-        <v>75</v>
-      </c>
-      <c r="AF4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH4" t="n">
-        <v>41</v>
-      </c>
-      <c r="AI4" t="n">
-        <v>42</v>
-      </c>
       <c r="AJ4" t="n">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="AK4" t="n">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="AL4" t="n">
         <v>0</v>
       </c>
       <c r="AM4" t="n">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="AN4" t="n">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="AO4" t="n">
         <v>0</v>
       </c>
       <c r="AP4" t="n">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="AQ4" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="AR4" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="AS4" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="AT4" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="AU4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV4" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="AW4" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="AX4" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="AY4" t="n">
         <v>0</v>
       </c>
       <c r="AZ4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA4" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="BB4" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="BC4" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="BD4" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE4" t="n">
+        <v>1</v>
+      </c>
+      <c r="BF4" t="n">
         <v>2</v>
       </c>
-      <c r="BE4" t="n">
-        <v>8</v>
-      </c>
-      <c r="BF4" t="n">
-        <v>12</v>
-      </c>
       <c r="BG4" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="BH4" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="BI4" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="BJ4" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="BK4" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="BL4" t="n">
         <v>1</v>
@@ -1527,19 +1527,19 @@
         <v>3</v>
       </c>
       <c r="BN4" t="n">
+        <v>2</v>
+      </c>
+      <c r="BO4" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP4" t="n">
         <v>3</v>
       </c>
-      <c r="BO4" t="n">
+      <c r="BQ4" t="n">
         <v>4</v>
       </c>
-      <c r="BP4" t="n">
-        <v>0</v>
-      </c>
-      <c r="BQ4" t="n">
-        <v>0</v>
-      </c>
       <c r="BR4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BS4" t="n">
         <v>0</v>
@@ -1548,20 +1548,20 @@
         <v>0</v>
       </c>
       <c r="BU4" t="n">
+        <v>0</v>
+      </c>
+      <c r="BV4" t="n">
+        <v>0</v>
+      </c>
+      <c r="BW4" t="n">
+        <v>0</v>
+      </c>
+      <c r="BX4" t="n">
+        <v>0</v>
+      </c>
+      <c r="BY4" t="n">
         <v>2</v>
       </c>
-      <c r="BV4" t="n">
-        <v>0</v>
-      </c>
-      <c r="BW4" t="n">
-        <v>1</v>
-      </c>
-      <c r="BX4" t="n">
-        <v>0</v>
-      </c>
-      <c r="BY4" t="n">
-        <v>0</v>
-      </c>
       <c r="BZ4" t="n">
         <v>0</v>
       </c>
@@ -1575,128 +1575,128 @@
         <v>0</v>
       </c>
       <c r="CD4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>E. coli</t>
+          <t>S. pneumoniae</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>5823</v>
+        <v>995</v>
       </c>
       <c r="C5" t="n">
-        <v>1830</v>
+        <v>852</v>
       </c>
       <c r="D5" t="n">
-        <v>892</v>
+        <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>224</v>
+        <v>123</v>
       </c>
       <c r="F5" t="n">
+        <v>17</v>
+      </c>
+      <c r="G5" t="n">
         <v>114</v>
       </c>
-      <c r="G5" t="n">
-        <v>783</v>
-      </c>
       <c r="H5" t="n">
-        <v>297</v>
+        <v>410</v>
       </c>
       <c r="I5" t="n">
-        <v>126</v>
+        <v>2</v>
       </c>
       <c r="J5" t="n">
-        <v>67</v>
+        <v>7</v>
       </c>
       <c r="K5" t="n">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>144</v>
+        <v>14</v>
       </c>
       <c r="M5" t="n">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="N5" t="n">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="O5" t="n">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="P5" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="Q5" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="R5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="S5" t="n">
+        <v>4</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" t="n">
+        <v>0</v>
+      </c>
+      <c r="V5" t="n">
+        <v>0</v>
+      </c>
+      <c r="W5" t="n">
+        <v>0</v>
+      </c>
+      <c r="X5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>8</v>
+      </c>
+      <c r="AG5" t="n">
         <v>5</v>
       </c>
-      <c r="T5" t="n">
-        <v>1</v>
-      </c>
-      <c r="U5" t="n">
-        <v>8</v>
-      </c>
-      <c r="V5" t="n">
-        <v>9</v>
-      </c>
-      <c r="W5" t="n">
-        <v>2</v>
-      </c>
-      <c r="X5" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y5" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z5" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA5" t="n">
-        <v>6</v>
-      </c>
-      <c r="AB5" t="n">
-        <v>4</v>
-      </c>
-      <c r="AC5" t="n">
-        <v>10</v>
-      </c>
-      <c r="AD5" t="n">
-        <v>3</v>
-      </c>
-      <c r="AE5" t="n">
-        <v>10</v>
-      </c>
-      <c r="AF5" t="n">
-        <v>7</v>
-      </c>
-      <c r="AG5" t="n">
-        <v>7</v>
-      </c>
       <c r="AH5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI5" t="n">
         <v>0</v>
       </c>
       <c r="AJ5" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="AK5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AL5" t="n">
         <v>0</v>
       </c>
       <c r="AM5" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="AN5" t="n">
         <v>0</v>
@@ -1705,10 +1705,10 @@
         <v>0</v>
       </c>
       <c r="AP5" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AQ5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR5" t="n">
         <v>0</v>
@@ -1729,10 +1729,10 @@
         <v>0</v>
       </c>
       <c r="AX5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ5" t="n">
         <v>0</v>
@@ -1765,7 +1765,7 @@
         <v>0</v>
       </c>
       <c r="BJ5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BK5" t="n">
         <v>0</v>
@@ -1777,7 +1777,7 @@
         <v>0</v>
       </c>
       <c r="BN5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BO5" t="n">
         <v>0</v>
@@ -1786,7 +1786,7 @@
         <v>1</v>
       </c>
       <c r="BQ5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR5" t="n">
         <v>0</v>
@@ -1831,135 +1831,135 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>H. pylori</t>
+          <t>S. aureus</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>912</v>
+        <v>337</v>
       </c>
       <c r="C6" t="n">
-        <v>476</v>
+        <v>879</v>
       </c>
       <c r="D6" t="n">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="E6" t="n">
-        <v>420</v>
+        <v>97</v>
       </c>
       <c r="F6" t="n">
-        <v>82</v>
+        <v>19</v>
       </c>
       <c r="G6" t="n">
-        <v>773</v>
+        <v>41</v>
       </c>
       <c r="H6" t="n">
-        <v>621</v>
+        <v>600</v>
       </c>
       <c r="I6" t="n">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="J6" t="n">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="K6" t="n">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="L6" t="n">
-        <v>108</v>
+        <v>2</v>
       </c>
       <c r="M6" t="n">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="N6" t="n">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="O6" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="P6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>1</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" t="n">
+        <v>10</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" t="n">
+        <v>0</v>
+      </c>
+      <c r="V6" t="n">
+        <v>0</v>
+      </c>
+      <c r="W6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>5</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>6</v>
+      </c>
+      <c r="AG6" t="n">
+        <v>5</v>
+      </c>
+      <c r="AH6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI6" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK6" t="n">
         <v>2</v>
       </c>
-      <c r="Q6" t="n">
+      <c r="AL6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP6" t="n">
         <v>2</v>
       </c>
-      <c r="R6" t="n">
-        <v>15</v>
-      </c>
-      <c r="S6" t="n">
-        <v>14</v>
-      </c>
-      <c r="T6" t="n">
-        <v>2</v>
-      </c>
-      <c r="U6" t="n">
-        <v>1</v>
-      </c>
-      <c r="V6" t="n">
-        <v>8</v>
-      </c>
-      <c r="W6" t="n">
-        <v>5</v>
-      </c>
-      <c r="X6" t="n">
+      <c r="AQ6" t="n">
         <v>3</v>
       </c>
-      <c r="Y6" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA6" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB6" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC6" t="n">
-        <v>6</v>
-      </c>
-      <c r="AD6" t="n">
-        <v>6</v>
-      </c>
-      <c r="AE6" t="n">
-        <v>6</v>
-      </c>
-      <c r="AF6" t="n">
-        <v>5</v>
-      </c>
-      <c r="AG6" t="n">
-        <v>6</v>
-      </c>
-      <c r="AH6" t="n">
-        <v>1</v>
-      </c>
-      <c r="AI6" t="n">
-        <v>4</v>
-      </c>
-      <c r="AJ6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK6" t="n">
-        <v>6</v>
-      </c>
-      <c r="AL6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM6" t="n">
-        <v>1</v>
-      </c>
-      <c r="AN6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP6" t="n">
-        <v>7</v>
-      </c>
-      <c r="AQ6" t="n">
-        <v>0</v>
-      </c>
       <c r="AR6" t="n">
         <v>0</v>
       </c>
@@ -1976,7 +1976,7 @@
         <v>0</v>
       </c>
       <c r="AW6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX6" t="n">
         <v>0</v>
@@ -1985,7 +1985,7 @@
         <v>0</v>
       </c>
       <c r="AZ6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA6" t="n">
         <v>0</v>
@@ -2000,10 +2000,10 @@
         <v>0</v>
       </c>
       <c r="BE6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF6" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BG6" t="n">
         <v>0</v>
@@ -2015,31 +2015,31 @@
         <v>0</v>
       </c>
       <c r="BJ6" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="BK6" t="n">
         <v>0</v>
       </c>
       <c r="BL6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM6" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BN6" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BO6" t="n">
         <v>0</v>
       </c>
       <c r="BP6" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BQ6" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="BR6" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BS6" t="n">
         <v>0</v>
@@ -2060,7 +2060,7 @@
         <v>0</v>
       </c>
       <c r="BY6" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BZ6" t="n">
         <v>0</v>
@@ -2331,224 +2331,224 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>S. cerevisiae</t>
+          <t>C. shaoxiangyii</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>4745</v>
+        <v>20456</v>
       </c>
       <c r="C8" t="n">
-        <v>2632</v>
+        <v>4947</v>
       </c>
       <c r="D8" t="n">
-        <v>105</v>
+        <v>8552</v>
       </c>
       <c r="E8" t="n">
-        <v>6350</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>404</v>
+        <v>2991</v>
       </c>
       <c r="G8" t="n">
-        <v>904</v>
+        <v>1621</v>
       </c>
       <c r="H8" t="n">
-        <v>2090</v>
+        <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>80</v>
+        <v>1814</v>
       </c>
       <c r="J8" t="n">
-        <v>239</v>
+        <v>1524</v>
       </c>
       <c r="K8" t="n">
-        <v>201</v>
+        <v>1258</v>
       </c>
       <c r="L8" t="n">
-        <v>137</v>
+        <v>987</v>
       </c>
       <c r="M8" t="n">
-        <v>52</v>
+        <v>803</v>
       </c>
       <c r="N8" t="n">
-        <v>592</v>
+        <v>306</v>
       </c>
       <c r="O8" t="n">
-        <v>22</v>
+        <v>484</v>
       </c>
       <c r="P8" t="n">
+        <v>394</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>301</v>
+      </c>
+      <c r="R8" t="n">
+        <v>32</v>
+      </c>
+      <c r="S8" t="n">
+        <v>4</v>
+      </c>
+      <c r="T8" t="n">
+        <v>262</v>
+      </c>
+      <c r="U8" t="n">
+        <v>188</v>
+      </c>
+      <c r="V8" t="n">
+        <v>193</v>
+      </c>
+      <c r="W8" t="n">
+        <v>145</v>
+      </c>
+      <c r="X8" t="n">
+        <v>103</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>117</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>122</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>91</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>81</v>
+      </c>
+      <c r="AC8" t="n">
+        <v>102</v>
+      </c>
+      <c r="AD8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE8" t="n">
+        <v>75</v>
+      </c>
+      <c r="AF8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH8" t="n">
+        <v>41</v>
+      </c>
+      <c r="AI8" t="n">
+        <v>42</v>
+      </c>
+      <c r="AJ8" t="n">
+        <v>27</v>
+      </c>
+      <c r="AK8" t="n">
+        <v>23</v>
+      </c>
+      <c r="AL8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM8" t="n">
+        <v>32</v>
+      </c>
+      <c r="AN8" t="n">
+        <v>32</v>
+      </c>
+      <c r="AO8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP8" t="n">
+        <v>16</v>
+      </c>
+      <c r="AQ8" t="n">
+        <v>11</v>
+      </c>
+      <c r="AR8" t="n">
+        <v>16</v>
+      </c>
+      <c r="AS8" t="n">
+        <v>20</v>
+      </c>
+      <c r="AT8" t="n">
+        <v>13</v>
+      </c>
+      <c r="AU8" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV8" t="n">
+        <v>11</v>
+      </c>
+      <c r="AW8" t="n">
+        <v>13</v>
+      </c>
+      <c r="AX8" t="n">
         <v>9</v>
       </c>
-      <c r="Q8" t="n">
+      <c r="AY8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ8" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA8" t="n">
+        <v>13</v>
+      </c>
+      <c r="BB8" t="n">
+        <v>10</v>
+      </c>
+      <c r="BC8" t="n">
+        <v>16</v>
+      </c>
+      <c r="BD8" t="n">
+        <v>2</v>
+      </c>
+      <c r="BE8" t="n">
         <v>8</v>
       </c>
-      <c r="R8" t="n">
-        <v>632</v>
-      </c>
-      <c r="S8" t="n">
-        <v>440</v>
-      </c>
-      <c r="T8" t="n">
-        <v>46</v>
-      </c>
-      <c r="U8" t="n">
-        <v>1</v>
-      </c>
-      <c r="V8" t="n">
-        <v>10</v>
-      </c>
-      <c r="W8" t="n">
-        <v>40</v>
-      </c>
-      <c r="X8" t="n">
+      <c r="BF8" t="n">
+        <v>12</v>
+      </c>
+      <c r="BG8" t="n">
+        <v>11</v>
+      </c>
+      <c r="BH8" t="n">
+        <v>9</v>
+      </c>
+      <c r="BI8" t="n">
+        <v>8</v>
+      </c>
+      <c r="BJ8" t="n">
+        <v>1</v>
+      </c>
+      <c r="BK8" t="n">
         <v>6</v>
       </c>
-      <c r="Y8" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC8" t="n">
-        <v>4</v>
-      </c>
-      <c r="AD8" t="n">
-        <v>189</v>
-      </c>
-      <c r="AE8" t="n">
-        <v>16</v>
-      </c>
-      <c r="AF8" t="n">
-        <v>24</v>
-      </c>
-      <c r="AG8" t="n">
-        <v>20</v>
-      </c>
-      <c r="AH8" t="n">
-        <v>27</v>
-      </c>
-      <c r="AI8" t="n">
-        <v>16</v>
-      </c>
-      <c r="AJ8" t="n">
-        <v>7</v>
-      </c>
-      <c r="AK8" t="n">
-        <v>8</v>
-      </c>
-      <c r="AL8" t="n">
-        <v>39</v>
-      </c>
-      <c r="AM8" t="n">
-        <v>5</v>
-      </c>
-      <c r="AN8" t="n">
-        <v>5</v>
-      </c>
-      <c r="AO8" t="n">
-        <v>31</v>
-      </c>
-      <c r="AP8" t="n">
-        <v>4</v>
-      </c>
-      <c r="AQ8" t="n">
-        <v>22</v>
-      </c>
-      <c r="AR8" t="n">
-        <v>1</v>
-      </c>
-      <c r="AS8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU8" t="n">
-        <v>25</v>
-      </c>
-      <c r="AV8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY8" t="n">
-        <v>15</v>
-      </c>
-      <c r="AZ8" t="n">
-        <v>16</v>
-      </c>
-      <c r="BA8" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB8" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC8" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD8" t="n">
-        <v>11</v>
-      </c>
-      <c r="BE8" t="n">
-        <v>0</v>
-      </c>
-      <c r="BF8" t="n">
-        <v>0</v>
-      </c>
-      <c r="BG8" t="n">
-        <v>0</v>
-      </c>
-      <c r="BH8" t="n">
-        <v>0</v>
-      </c>
-      <c r="BI8" t="n">
-        <v>0</v>
-      </c>
-      <c r="BJ8" t="n">
-        <v>1</v>
-      </c>
-      <c r="BK8" t="n">
-        <v>0</v>
-      </c>
       <c r="BL8" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="BM8" t="n">
         <v>3</v>
       </c>
       <c r="BN8" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BO8" t="n">
         <v>4</v>
       </c>
       <c r="BP8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ8" t="n">
         <v>0</v>
       </c>
       <c r="BR8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU8" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BV8" t="n">
         <v>0</v>
@@ -2563,230 +2563,230 @@
         <v>0</v>
       </c>
       <c r="BZ8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA8" t="n">
         <v>0</v>
       </c>
       <c r="CB8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC8" t="n">
         <v>0</v>
       </c>
       <c r="CD8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>S. aureus</t>
+          <t>E. coli</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>337</v>
+        <v>5823</v>
       </c>
       <c r="C9" t="n">
-        <v>879</v>
+        <v>1830</v>
       </c>
       <c r="D9" t="n">
+        <v>892</v>
+      </c>
+      <c r="E9" t="n">
+        <v>224</v>
+      </c>
+      <c r="F9" t="n">
+        <v>114</v>
+      </c>
+      <c r="G9" t="n">
+        <v>783</v>
+      </c>
+      <c r="H9" t="n">
+        <v>297</v>
+      </c>
+      <c r="I9" t="n">
+        <v>126</v>
+      </c>
+      <c r="J9" t="n">
+        <v>67</v>
+      </c>
+      <c r="K9" t="n">
+        <v>29</v>
+      </c>
+      <c r="L9" t="n">
+        <v>144</v>
+      </c>
+      <c r="M9" t="n">
+        <v>23</v>
+      </c>
+      <c r="N9" t="n">
+        <v>16</v>
+      </c>
+      <c r="O9" t="n">
+        <v>24</v>
+      </c>
+      <c r="P9" t="n">
+        <v>18</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>15</v>
+      </c>
+      <c r="R9" t="n">
+        <v>3</v>
+      </c>
+      <c r="S9" t="n">
+        <v>5</v>
+      </c>
+      <c r="T9" t="n">
+        <v>1</v>
+      </c>
+      <c r="U9" t="n">
+        <v>8</v>
+      </c>
+      <c r="V9" t="n">
+        <v>9</v>
+      </c>
+      <c r="W9" t="n">
+        <v>2</v>
+      </c>
+      <c r="X9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>6</v>
+      </c>
+      <c r="AB9" t="n">
+        <v>4</v>
+      </c>
+      <c r="AC9" t="n">
+        <v>10</v>
+      </c>
+      <c r="AD9" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE9" t="n">
+        <v>10</v>
+      </c>
+      <c r="AF9" t="n">
         <v>7</v>
       </c>
-      <c r="E9" t="n">
-        <v>97</v>
-      </c>
-      <c r="F9" t="n">
-        <v>19</v>
-      </c>
-      <c r="G9" t="n">
-        <v>41</v>
-      </c>
-      <c r="H9" t="n">
-        <v>600</v>
-      </c>
-      <c r="I9" t="n">
+      <c r="AG9" t="n">
+        <v>7</v>
+      </c>
+      <c r="AH9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ9" t="n">
+        <v>7</v>
+      </c>
+      <c r="AK9" t="n">
+        <v>3</v>
+      </c>
+      <c r="AL9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM9" t="n">
+        <v>9</v>
+      </c>
+      <c r="AN9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP9" t="n">
+        <v>4</v>
+      </c>
+      <c r="AQ9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AY9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AZ9" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA9" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB9" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC9" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD9" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE9" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF9" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG9" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH9" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI9" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ9" t="n">
         <v>2</v>
       </c>
-      <c r="J9" t="n">
-        <v>68</v>
-      </c>
-      <c r="K9" t="n">
-        <v>3</v>
-      </c>
-      <c r="L9" t="n">
+      <c r="BK9" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL9" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM9" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN9" t="n">
         <v>2</v>
       </c>
-      <c r="M9" t="n">
-        <v>0</v>
-      </c>
-      <c r="N9" t="n">
-        <v>48</v>
-      </c>
-      <c r="O9" t="n">
-        <v>0</v>
-      </c>
-      <c r="P9" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q9" t="n">
-        <v>1</v>
-      </c>
-      <c r="R9" t="n">
-        <v>0</v>
-      </c>
-      <c r="S9" t="n">
-        <v>10</v>
-      </c>
-      <c r="T9" t="n">
-        <v>0</v>
-      </c>
-      <c r="U9" t="n">
-        <v>0</v>
-      </c>
-      <c r="V9" t="n">
-        <v>0</v>
-      </c>
-      <c r="W9" t="n">
-        <v>0</v>
-      </c>
-      <c r="X9" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y9" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD9" t="n">
-        <v>5</v>
-      </c>
-      <c r="AE9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF9" t="n">
-        <v>6</v>
-      </c>
-      <c r="AG9" t="n">
-        <v>5</v>
-      </c>
-      <c r="AH9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI9" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK9" t="n">
-        <v>2</v>
-      </c>
-      <c r="AL9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP9" t="n">
-        <v>2</v>
-      </c>
-      <c r="AQ9" t="n">
-        <v>3</v>
-      </c>
-      <c r="AR9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AV9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AZ9" t="n">
-        <v>0</v>
-      </c>
-      <c r="BA9" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB9" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC9" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD9" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE9" t="n">
-        <v>0</v>
-      </c>
-      <c r="BF9" t="n">
-        <v>0</v>
-      </c>
-      <c r="BG9" t="n">
-        <v>0</v>
-      </c>
-      <c r="BH9" t="n">
-        <v>0</v>
-      </c>
-      <c r="BI9" t="n">
-        <v>0</v>
-      </c>
-      <c r="BJ9" t="n">
-        <v>0</v>
-      </c>
-      <c r="BK9" t="n">
-        <v>0</v>
-      </c>
-      <c r="BL9" t="n">
-        <v>0</v>
-      </c>
-      <c r="BM9" t="n">
-        <v>0</v>
-      </c>
-      <c r="BN9" t="n">
-        <v>0</v>
-      </c>
       <c r="BO9" t="n">
         <v>0</v>
       </c>
       <c r="BP9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BQ9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BR9" t="n">
         <v>0</v>
@@ -2831,207 +2831,207 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>S. pneumoniae</t>
+          <t>S. cerevisiae</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>995</v>
+        <v>4745</v>
       </c>
       <c r="C10" t="n">
-        <v>852</v>
+        <v>2632</v>
       </c>
       <c r="D10" t="n">
+        <v>105</v>
+      </c>
+      <c r="E10" t="n">
+        <v>6350</v>
+      </c>
+      <c r="F10" t="n">
+        <v>404</v>
+      </c>
+      <c r="G10" t="n">
+        <v>904</v>
+      </c>
+      <c r="H10" t="n">
+        <v>2090</v>
+      </c>
+      <c r="I10" t="n">
+        <v>80</v>
+      </c>
+      <c r="J10" t="n">
+        <v>239</v>
+      </c>
+      <c r="K10" t="n">
+        <v>201</v>
+      </c>
+      <c r="L10" t="n">
+        <v>137</v>
+      </c>
+      <c r="M10" t="n">
+        <v>52</v>
+      </c>
+      <c r="N10" t="n">
+        <v>592</v>
+      </c>
+      <c r="O10" t="n">
+        <v>22</v>
+      </c>
+      <c r="P10" t="n">
+        <v>9</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>8</v>
+      </c>
+      <c r="R10" t="n">
+        <v>632</v>
+      </c>
+      <c r="S10" t="n">
+        <v>440</v>
+      </c>
+      <c r="T10" t="n">
+        <v>46</v>
+      </c>
+      <c r="U10" t="n">
+        <v>1</v>
+      </c>
+      <c r="V10" t="n">
         <v>10</v>
       </c>
-      <c r="E10" t="n">
-        <v>123</v>
-      </c>
-      <c r="F10" t="n">
-        <v>17</v>
-      </c>
-      <c r="G10" t="n">
-        <v>114</v>
-      </c>
-      <c r="H10" t="n">
-        <v>410</v>
-      </c>
-      <c r="I10" t="n">
-        <v>2</v>
-      </c>
-      <c r="J10" t="n">
+      <c r="W10" t="n">
+        <v>40</v>
+      </c>
+      <c r="X10" t="n">
+        <v>6</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC10" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD10" t="n">
+        <v>189</v>
+      </c>
+      <c r="AE10" t="n">
+        <v>16</v>
+      </c>
+      <c r="AF10" t="n">
+        <v>24</v>
+      </c>
+      <c r="AG10" t="n">
+        <v>20</v>
+      </c>
+      <c r="AH10" t="n">
+        <v>27</v>
+      </c>
+      <c r="AI10" t="n">
+        <v>16</v>
+      </c>
+      <c r="AJ10" t="n">
         <v>7</v>
       </c>
-      <c r="K10" t="n">
-        <v>0</v>
-      </c>
-      <c r="L10" t="n">
-        <v>14</v>
-      </c>
-      <c r="M10" t="n">
+      <c r="AK10" t="n">
+        <v>8</v>
+      </c>
+      <c r="AL10" t="n">
+        <v>39</v>
+      </c>
+      <c r="AM10" t="n">
+        <v>5</v>
+      </c>
+      <c r="AN10" t="n">
+        <v>5</v>
+      </c>
+      <c r="AO10" t="n">
+        <v>31</v>
+      </c>
+      <c r="AP10" t="n">
+        <v>4</v>
+      </c>
+      <c r="AQ10" t="n">
+        <v>22</v>
+      </c>
+      <c r="AR10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU10" t="n">
+        <v>25</v>
+      </c>
+      <c r="AV10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY10" t="n">
+        <v>15</v>
+      </c>
+      <c r="AZ10" t="n">
+        <v>16</v>
+      </c>
+      <c r="BA10" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB10" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC10" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD10" t="n">
+        <v>11</v>
+      </c>
+      <c r="BE10" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF10" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG10" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH10" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI10" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ10" t="n">
+        <v>1</v>
+      </c>
+      <c r="BK10" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL10" t="n">
+        <v>7</v>
+      </c>
+      <c r="BM10" t="n">
         <v>3</v>
       </c>
-      <c r="N10" t="n">
-        <v>34</v>
-      </c>
-      <c r="O10" t="n">
-        <v>1</v>
-      </c>
-      <c r="P10" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>0</v>
-      </c>
-      <c r="R10" t="n">
-        <v>1</v>
-      </c>
-      <c r="S10" t="n">
+      <c r="BN10" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO10" t="n">
         <v>4</v>
       </c>
-      <c r="T10" t="n">
-        <v>0</v>
-      </c>
-      <c r="U10" t="n">
-        <v>0</v>
-      </c>
-      <c r="V10" t="n">
-        <v>0</v>
-      </c>
-      <c r="W10" t="n">
-        <v>0</v>
-      </c>
-      <c r="X10" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y10" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD10" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE10" t="n">
-        <v>1</v>
-      </c>
-      <c r="AF10" t="n">
-        <v>8</v>
-      </c>
-      <c r="AG10" t="n">
-        <v>5</v>
-      </c>
-      <c r="AH10" t="n">
-        <v>1</v>
-      </c>
-      <c r="AI10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ10" t="n">
-        <v>1</v>
-      </c>
-      <c r="AK10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ10" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AV10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AZ10" t="n">
-        <v>0</v>
-      </c>
-      <c r="BA10" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB10" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC10" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD10" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE10" t="n">
-        <v>0</v>
-      </c>
-      <c r="BF10" t="n">
-        <v>0</v>
-      </c>
-      <c r="BG10" t="n">
-        <v>0</v>
-      </c>
-      <c r="BH10" t="n">
-        <v>0</v>
-      </c>
-      <c r="BI10" t="n">
-        <v>0</v>
-      </c>
-      <c r="BJ10" t="n">
-        <v>0</v>
-      </c>
-      <c r="BK10" t="n">
-        <v>0</v>
-      </c>
-      <c r="BL10" t="n">
-        <v>0</v>
-      </c>
-      <c r="BM10" t="n">
-        <v>0</v>
-      </c>
-      <c r="BN10" t="n">
-        <v>0</v>
-      </c>
-      <c r="BO10" t="n">
-        <v>0</v>
-      </c>
       <c r="BP10" t="n">
         <v>1</v>
       </c>
@@ -3039,13 +3039,13 @@
         <v>0</v>
       </c>
       <c r="BR10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BS10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BT10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BU10" t="n">
         <v>0</v>
@@ -3054,7 +3054,7 @@
         <v>0</v>
       </c>
       <c r="BW10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BX10" t="n">
         <v>0</v>
@@ -3063,13 +3063,13 @@
         <v>0</v>
       </c>
       <c r="BZ10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CA10" t="n">
         <v>0</v>
       </c>
       <c r="CB10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CC10" t="n">
         <v>0</v>

</xml_diff>